<commit_message>
ccdc resource page only
</commit_message>
<xml_diff>
--- a/InputFiles/CCDC_Datasets_20230413.xlsx
+++ b/InputFiles/CCDC_Datasets_20230413.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B078E1C1-E21B-40F7-BDA6-E2289FBD3B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA535235-16E9-4398-A4F6-6FA9C5F4A69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -232,7 +232,7 @@
     <t>elliot.stieglitz@ucsf.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1002/pbc.25342 ; https://doi.org/10.1038/ng.3400 ; https://doi.org/10.1038/s41467-017-02178-9 ; https://doi.org/10.1002/pbc.27034 ; https://doi.org/10.1002/pbc.27948</t>
+    <t>https://doi.org/10.1002/pbc.25342 https://doi.org/10.1038/ng.3400 https://doi.org/10.1038/s41467-017-02178-9 https://doi.org/10.1002/pbc.27034 https://doi.org/10.1002/pbc.27948</t>
   </si>
   <si>
     <t>188</t>
@@ -793,7 +793,7 @@
     <t>Malachi Griffith, PhD ; Obi Griffith, PhD</t>
   </si>
   <si>
-    <t>mgriffit@wustl.edu ; obigriffith@wustl.edu</t>
+    <t>mgriffit@wustl.edu , obigriffith@wustl.edu</t>
   </si>
   <si>
     <t>https://doi.org/10.1038/ng.3774</t>
@@ -910,7 +910,7 @@
     <t>RNA Sequencing (35); Whole Exome Sequencing (59); Whole Genome Sequencing (13)</t>
   </si>
   <si>
-    <t>phs000694;phs000699</t>
+    <t>phs000694 phs000699</t>
   </si>
   <si>
     <t>U01CA105423|Exploiting mouse models of pediatric cancers and epigenetics for therapy</t>
@@ -979,7 +979,7 @@
     <t>Rhabdomyosarcoma (RMS) is the most common soft tissue sarcoma of childhood accounting for approximately 350 newly diagnosed cases yearly in the United States. With the development of multimodal chemotherapy regimens, relapse-free survival rates have improved to 70-80% in patients with localized disease albeit with significant toxicity. Unfortunately, despite aggressive treatment, patients with metastatic or recurrent disease continue to suffer from high mortality. Further characterization of the genetic events underlying this tumor type is critical for the development of more effective diagnostic, prognostic and therapeutic strategies. In a collaborative effort between the National Cancer Institute, the Children's Oncology Group, and the Broad Institute, we use a combination of whole-genome and whole-exome sequencing to characterize the landscape of somatic alterations in tumor/normal pairs.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1158/2159-8290.CD-13-0639 ; https://doi.org/10.1200/PO.20.00218</t>
+    <t>https://doi.org/10.1158/2159-8290.CD-13-0639 https://doi.org/10.1200/PO.20.00218</t>
   </si>
   <si>
     <t>147</t>
@@ -1069,7 +1069,7 @@
     <t>simon@rockefeller.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1126/science.1249484 ; https://doi.org/10.1073/pnas.1424894112 ; https://doi.org/10.18632/oncotarget.2712</t>
+    <t>https://doi.org/10.1126/science.1249484 https://doi.org/10.1073/pnas.1424894112 https://doi.org/10.18632/oncotarget.2712</t>
   </si>
   <si>
     <t>9</t>
@@ -1177,7 +1177,7 @@
     <t>splon@bcm.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1186/s13073-014-0069-3 ; https://doi.org/10.1001/jamaoncol.2015.5699</t>
+    <t>https://doi.org/10.1186/s13073-014-0069-3 https://doi.org/10.1001/jamaoncol.2015.5699</t>
   </si>
   <si>
     <t>253</t>
@@ -1195,7 +1195,7 @@
     <t>Female (123); Male (130)</t>
   </si>
   <si>
-    <t>phs001026;phs001878</t>
+    <t>phs001026 phs001878</t>
   </si>
   <si>
     <t>U01HG006485|Incorporation of Genomic Sequencing into Pediatric Cancer Care</t>
@@ -1273,7 +1273,7 @@
     <t>maris@chop.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1002/ijc.31822 ; https://doi.org/10.1111/jcmm.13226</t>
+    <t>https://doi.org/10.1002/ijc.31822 https://doi.org/10.1111/jcmm.13226</t>
   </si>
   <si>
     <t>5,000</t>
@@ -1318,7 +1318,7 @@
     <t>charles.mullighan@stjude.org</t>
   </si>
   <si>
-    <t>https://doi.org/10.1038/nmeth.1628 ; https://doi.org/10.1038/nature10725</t>
+    <t>https://doi.org/10.1038/nmeth.1628 https://doi.org/10.1038/nature10725</t>
   </si>
   <si>
     <t>106</t>
@@ -1915,7 +1915,7 @@
     <t>We estimated the plasma clearance of methotrexate from 1279 acute lymphoblastic leukemia (ALL) patients treated on the Children Oncology Group 9904 and 9905 trials. Patients received either a 24-hour infusion of a 1 g/m2 dose or 4-hour infusion of a 2 g/m2 dose). Methotrexate clearance was lower in older children (p=7 x 10-7), females (p=2.7 x 10-4), and patients who received a delayed intensification phase (p=0.0022). In a genome-wide analysis, methotrexate clearance was associated with polymorphisms in the SLCO1B1 gene (p=2.1 x 10-11), which encodes for an organic anion transporter. This replicates findings using different schedules of high-dose methotrexate in ALL patients treated on St. Jude protocols. A combined meta-analysis yields a p-value of 5.7 x 10-19 for the association of methotrexate clearance with SLCO1B1 SNP rs4149056. This dataset includes the dependent variable of methotrexate clearance and all of the SNP data available from arrays.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1101/gr.129668.111 ; https://doi.org/10.1200/jco.2008.20.4156 ; https://doi.org/10.1182/blood-2012-08-452839</t>
+    <t>https://doi.org/10.1101/gr.129668.111 https://doi.org/10.1200/jco.2008.20.4156 https://doi.org/10.1182/blood-2012-08-452839</t>
   </si>
   <si>
     <t>1,279</t>
@@ -1957,7 +1957,7 @@
     <t>Using risk-directed therapy for childhood acute lymphoblastic leukemia (ALL), outcome has improved dramatically in the last 40 years. However, a substantial portion of patients experience relapse, many of whom have no known risk factors. Taking a genome-wide approach, we sought to evaluate the relationships between germline SNP genotypes and the risk of relapse in 2,535 children with newly diagnosed ALL after adjusting for genetic ancestry and treatment regimen. We examine prognostic value of selected SNPs in the context of known relapse risk factors (molecular subtypes, minimal residual disease, age and leukocyte count at diagnosis). Associations of relapse-related SNPs with pharmacokinetic and pharmacodynamics of antileukemic drugs offer plausible mechanism by which they are linked to treatment outcome. Finally, we aim to identify SNPs that are related to both genetic ancestry and relapse which are likely to contribute to racial disparities in ALL survival.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1182/blood-2012-07-440107 ; https://doi.org/10.1038/ng.763</t>
+    <t>https://doi.org/10.1182/blood-2012-07-440107 https://doi.org/10.1038/ng.763</t>
   </si>
   <si>
     <t>2,487</t>
@@ -2293,7 +2293,7 @@
     <t>The Center for Cancer Research (CCR), of the intramural NCI undertook a multidimensional clinical genomics study of children and adolescent young adults with relapsed and refractory cancers who were enrolled on other therapeutic trials to determine the feasibility of a genome guided precision therapy protocol in these patients.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1371/journal.pgen.1004475 ; https://doi.org/10.1158/2159-8290.cd-13-0639 ; https://doi.org/10.1158/1078-0432.ccr-15-2717</t>
+    <t>https://doi.org/10.1371/journal.pgen.1004475 https://doi.org/10.1158/2159-8290.cd-13-0639 https://doi.org/10.1158/1078-0432.ccr-15-2717</t>
   </si>
   <si>
     <t>83</t>
@@ -2434,7 +2434,7 @@
     <t>ann.moormann@umassmed.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1158/1541-7786.mcr-16-0305 ; https://doi.org/10.1002/ijc.30170</t>
+    <t>https://doi.org/10.1158/1541-7786.mcr-16-0305 https://doi.org/10.1002/ijc.30170</t>
   </si>
   <si>
     <t>39</t>
@@ -2482,7 +2482,7 @@
     <t>knathans@mail.med.upenn.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1038/ng.393 ; https://doi.org/10.1038/ng.3896 ; https://doi.org/10.1038/ng.3879 ; https://doi.org/10.1093/hmg/ddr207</t>
+    <t>https://doi.org/10.1038/ng.393 https://doi.org/10.1038/ng.3896 https://doi.org/10.1038/ng.3879 https://doi.org/10.1093/hmg/ddr207</t>
   </si>
   <si>
     <t>10,608</t>
@@ -2620,7 +2620,7 @@
     <t>mbulaits@mail.nih.gov</t>
   </si>
   <si>
-    <t>https://doi.org/10.1016/j.ebiom.2017.09.037 ; https://doi.org/10.1038/nature11378 ; https://doi.org/10.1002/ijc.23800</t>
+    <t>https://doi.org/10.1016/j.ebiom.2017.09.037 https://doi.org/10.1038/nature11378 https://doi.org/10.1002/ijc.23800</t>
   </si>
   <si>
     <t>568</t>
@@ -2752,7 +2752,7 @@
     <t>catherine.cottrell@nationwidechildrens.org</t>
   </si>
   <si>
-    <t>https://doi.org/10.3324/haematol.2019.231928 ; https://doi.org/10.1016/j.isci.2019.05.037 ; https://doi.org/10.1093/jnen/nlz093 ; https://doi.org/10.1101/mcs.a002618</t>
+    <t>https://doi.org/10.3324/haematol.2019.231928 https://doi.org/10.1016/j.isci.2019.05.037 https://doi.org/10.1093/jnen/nlz093 https://doi.org/10.1101/mcs.a002618</t>
   </si>
   <si>
     <t>259</t>
@@ -2989,7 +2989,7 @@
     <t>barrfg@nih.mail.gov</t>
   </si>
   <si>
-    <t>https://doi.org/10.1002/ijc.32006 ; https://doi.org/10.1038/modpathol.2015.82</t>
+    <t>https://doi.org/10.1002/ijc.32006 https://doi.org/10.1038/modpathol.2015.82</t>
   </si>
   <si>
     <t>134</t>
@@ -3127,7 +3127,7 @@
     <t>song.yao@roswellpark.org</t>
   </si>
   <si>
-    <t>https://doi.org/10.1016/s1470-2045(15)00363-0 ; https://doi.org/10.1002/pbc.26871 ; https://doi.org/10.1182/bloodadvances.2020003060</t>
+    <t>https://doi.org/10.1016/s1470-2045(15)00363-0 https://doi.org/10.1002/pbc.26871 https://doi.org/10.1182/bloodadvances.2020003060</t>
   </si>
   <si>
     <t>415</t>
@@ -3349,7 +3349,7 @@
     <t>James Amatruda, PhD</t>
   </si>
   <si>
-    <t>https://doi.org/10.1016/j.devcel.2019.11.007 ; https://doi.org/10.1111/andr.12644</t>
+    <t>https://doi.org/10.1016/j.devcel.2019.11.007 https://doi.org/10.1111/andr.12644</t>
   </si>
   <si>
     <t>94</t>
@@ -3592,7 +3592,7 @@
     <t>briand_crompton@dfci.harvard.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1002/cncr.32204 ; https://doi.org/10.1200/jco.2009.22.3768</t>
+    <t>https://doi.org/10.1002/cncr.32204 https://doi.org/10.1200/jco.2009.22.3768</t>
   </si>
   <si>
     <t>124</t>
@@ -3643,7 +3643,7 @@
     <t>william.carroll@nyulangone.org</t>
   </si>
   <si>
-    <t>https://doi.org/10.1158/1541-7786.mcr-20-0092 ; https://doi.org/10.1101/2022.02.24.481835</t>
+    <t>https://doi.org/10.1158/1541-7786.mcr-20-0092 https://doi.org/10.1101/2022.02.24.481835</t>
   </si>
   <si>
     <t>Acute Lymphoblastic Leukemia (6)</t>
@@ -3979,7 +3979,7 @@
     <t>The Beat AML program involved 11 academic medical centers who worked collectively to accrue a cohort of ~950 AML patient specimens and 11 pharmaceutical and biotechnology companies, who supplied drugs for testing. These specimens were subjected to whole exome sequencing, RNA-sequencing, and ex vivo drug sensitivity analyses.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1038/s41586-018-0623-z ; https://doi.org/10.1038/s41467-018-08263-x</t>
+    <t>https://doi.org/10.1038/s41586-018-0623-z https://doi.org/10.1038/s41467-018-08263-x</t>
   </si>
   <si>
     <t>phs001657</t>
@@ -4120,7 +4120,7 @@
     <t>The Human Cancer Models Initiative (HCMI) is an international consortium that is generating novel, next-generation, tumor-derived culture models annotated with genomic and clinical data.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1158/2159-8290.CD-NB2016-103 ; https://doi.org/10.1080/15592294.2020.1762398</t>
+    <t>https://doi.org/10.1158/2159-8290.CD-NB2016-103 https://doi.org/10.1080/15592294.2020.1762398</t>
   </si>
   <si>
     <t>313</t>
@@ -4261,7 +4261,7 @@
     <t>rokita@email.chop.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1038/sdata.2017.33 ; https://doi.org/10.1016/j.celrep.2021.110047</t>
+    <t>https://doi.org/10.1038/sdata.2017.33 https://doi.org/10.1016/j.celrep.2021.110047</t>
   </si>
   <si>
     <t>Neuroblastoma (39)</t>
@@ -4291,7 +4291,7 @@
     <t>We used SNP arrays to perform genome-wide profiling of commonly-used neuroblastoma cell lines.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1038/sdata.2017.33 ; https://doi.org/10.1038/s41597-020-0458-y</t>
+    <t>https://doi.org/10.1038/sdata.2017.33 https://doi.org/10.1038/s41597-020-0458-y</t>
   </si>
   <si>
     <t>27</t>
@@ -4423,7 +4423,7 @@
     <t>hazel.rogers@nottingham.ac.uk</t>
   </si>
   <si>
-    <t>https://doi.org/10.1038/bjc.2013.170 ; https://doi.org/10.1158/0008-5472.can-13-1299</t>
+    <t>https://doi.org/10.1038/bjc.2013.170 https://doi.org/10.1158/0008-5472.can-13-1299</t>
   </si>
   <si>
     <t>24</t>
@@ -5002,7 +5002,7 @@
     <t>rogojina@uthscsa.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1038/nprot.2007.25 ; https://doi.org/10.1158/1078-0432.ccr-07-5090 ; https://doi.org/10.1002/pbc.21078</t>
+    <t>https://doi.org/10.1038/nprot.2007.25 https://doi.org/10.1158/1078-0432.ccr-07-5090 https://doi.org/10.1002/pbc.21078</t>
   </si>
   <si>
     <t>59</t>
@@ -5215,7 +5215,7 @@
     <t>dcc-support@icgc.org</t>
   </si>
   <si>
-    <t>https://doi.org/10.1038/nature11284 ; https://doi.org/10.1038/nature11327</t>
+    <t>https://doi.org/10.1038/nature11284 https://doi.org/10.1038/nature11327</t>
   </si>
   <si>
     <t>500</t>
@@ -5329,7 +5329,7 @@
     <t>This project is a collaboration with the trans-NIH Investigation of Co-occurring conditions across the Lifespan to Understand Down syndromE (INCLUDE) Project, which seeks to improve health and quality-of-life for individuals with Down syndrome, and NHLBI's TransOmics for Precision Medicine (TOPMed) program, which seeks to apply omics technologies to improve scientific understanding of the fundamental biological processes that underlie heart, lung, blood, and sleep (HLBS) disorders.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1182/blood.2018890764 ; https://doi.org/10.1534/g3.117.300366 ; https://doi.org/10.1352/1944-7558-123.6.514</t>
+    <t>https://doi.org/10.1182/blood.2018890764 https://doi.org/10.1534/g3.117.300366 https://doi.org/10.1352/1944-7558-123.6.514</t>
   </si>
   <si>
     <t>2,129</t>
@@ -5929,7 +5929,7 @@
     <t>ncichildhoodcancerdatainitiative@mail.nih.gov</t>
   </si>
   <si>
-    <t>https://github.com/PediatricOpenTargets/OpenPedCan-analysis ; https://cbtn.org</t>
+    <t>https://github.com/PediatricOpenTargets/OpenPedCan-analysis https://cbtn.org</t>
   </si>
   <si>
     <t>dataset/MyPART-MyPART</t>
@@ -6103,7 +6103,7 @@
     <t>RNA Sequencing (935); Whole Exome Sequencing (569); Whole Genome Sequencing (192)</t>
   </si>
   <si>
-    <t>phs000466;phs000467;phs000468;phs000720;phs000768;phs001052;phs001928</t>
+    <t>phs000466 phs000467 phs000468 phs000720 phs000768 phs001052 phs001928</t>
   </si>
   <si>
     <t>dataset/Oncogenomics-TMB_Immune_Landscape_Glioma</t>
@@ -6362,7 +6362,7 @@
     <t>https://www.pdxnetwork.org/contact</t>
   </si>
   <si>
-    <t>https://doi.org/10.1158/0008-5472.can-17-0582 ; https://doi.org/10.1093/narcan/zcac014</t>
+    <t>https://doi.org/10.1158/0008-5472.can-17-0582 https://doi.org/10.1093/narcan/zcac014</t>
   </si>
   <si>
     <t>Adenocarcinoma (10); Breast cancer, NOS (1); Cholangiocarcinoma (2); Invasive breast carcinoma (20); Malignant peripheral nerve sheath tumor (2); Melanoma (2); Non-rhabdomyosarcoma soft tissue sarcoma (1); Papillary thyroid carcinoma (1)</t>
@@ -6398,7 +6398,7 @@
     <t>The PDXNet Portal PDMR Data summarizes DNA and RNA sequencing files uploaded to the Cancer Genomics Cloud from the NCI Patient-Derived Model Repository (PDMR). This dataset consists of participants under the age of 40 years old.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1093/narcan/zcac014 ; https://doi.org/10.1186/s12967-021-02936-w</t>
+    <t>https://doi.org/10.1093/narcan/zcac014 https://doi.org/10.1186/s12967-021-02936-w</t>
   </si>
   <si>
     <t>1,174</t>
@@ -6440,7 +6440,7 @@
     <t>cerami@jimmy.harvard.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1126/scisignal.2004088 ; https://doi.org/10.1158/2159-8290.CD-12-0095</t>
+    <t>https://doi.org/10.1126/scisignal.2004088 https://doi.org/10.1158/2159-8290.CD-12-0095</t>
   </si>
   <si>
     <t>15,796</t>
@@ -6512,7 +6512,7 @@
     <t>smithm@ctep.nci.nih.gov</t>
   </si>
   <si>
-    <t>https://doi.org/10.1016/j.celrep.2019.09.071 ; https://doi.org/10.1002/pbc.29304 ; https://doi.org/10.1158/1535-7163.MCT-20-0406</t>
+    <t>https://doi.org/10.1016/j.celrep.2019.09.071 https://doi.org/10.1002/pbc.29304 https://doi.org/10.1158/1535-7163.MCT-20-0406</t>
   </si>
   <si>
     <t>244</t>
@@ -6998,7 +6998,7 @@
     <t>Clay McLeod ; Jinghui Zhang</t>
   </si>
   <si>
-    <t>Clay.McLeod@stjude.org ; jinghui.zhang@stjude.org</t>
+    <t>Clay.McLeod@stjude.org , jinghui.zhang@stjude.org</t>
   </si>
   <si>
     <t>https://doi.org/10.1038/ng.2287</t>
@@ -7286,7 +7286,7 @@
     <t>The Pan-Acute Lymphoblastic Leukemia (PanALL) dataset comprises cases of B-progenitor and T-lineage ALL encompassing the spectrum of ALL subtypes across the age continuum. Samples sequenced were obtained from multiple sites, centers and cooperative groups including St Jude Children's Research Hospital, The Children's Oncology Group, The Alliance-Cancer and Leukemia Group B, City of Hope National Medical Center, the Eastern Cooperative Oncology Group, MD Anderson Cancer Center, Northern Italy Leukemia Group, Princess Margaret Cancer Center, The Southwestern Oncology group, and UKALL.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1038/ng.2532 ; https://doi.org/10.1056/nejmoa1403088 ; https://doi.org/10.1038/ng.3909</t>
+    <t>https://doi.org/10.1038/ng.2532 https://doi.org/10.1056/nejmoa1403088 https://doi.org/10.1038/ng.3909</t>
   </si>
   <si>
     <t>735</t>
@@ -8021,7 +8021,7 @@
     <t>This collection contains data from the Children's Oncology Group (COG) Clinical Trial NCT00945009. Study Chair: Peter F. Ehrlich, M.D. M.S.C. It was sponsored by NCI and performed by the Children's Oncology Group under study number AREN0534. This phase III trial studies how well combination chemotherapy and surgery work in treating young patients with Wilms tumor. Drugs used in chemotherapy work in different ways to stop the growth of tumor cells, either by killing the cells, by stopping them from dividing, or by stopping them from spreading. Giving more than one drug (combination chemotherapy) may kill more tumor cells. Giving combination chemotherapy before surgery may make the tumor smaller and reduce the amount of normal tissue that needs to be removed. Giving it after surgery may kill any tumor cells that remain after surgery.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1097/sla.0000000000002356 ; https://doi.org/10.1002/cncr.32958</t>
+    <t>https://doi.org/10.1097/sla.0000000000002356 https://doi.org/10.1002/cncr.32958</t>
   </si>
   <si>
     <t>249</t>
@@ -8087,7 +8087,7 @@
     <t>This collection contains data from the Children's Oncology Group (COG) Clinical Trial NCT00379340. It was sponsored by NCI and performed by the Children's Oncology Group under study number AREN0533. This phase III trial is studying how well combination chemotherapy with or without radiation therapy works in treating young patients with newly diagnosed stage III or stage IV Favorable Histology Wilms' tumor. Drugs used in chemotherapy work in different ways to stop the growth of tumor cells, either by killing the cells or by stopping them from dividing. Radiation therapy uses high-energy x-rays to kill tumor cells. Giving more than one drug (combination chemotherapy) with or without radiation therapy may kill more tumor cells.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1200/jco.2017.77.1931 ; https://doi.org/10.1200/jco.18.01972</t>
+    <t>https://doi.org/10.1200/jco.2017.77.1931 https://doi.org/10.1200/jco.18.01972</t>
   </si>
   <si>
     <t>380</t>
@@ -8123,7 +8123,7 @@
     <t>This collection contains data from the Children's Oncology Group (COG) Clinical Trial NCT00352534. Principal Investigator: Conrad Fernandez, MD in Halifax, NS.  It was sponsored by NCI and performed by the Children's Oncology Group under study number AREN0532. This phase III trial is studying vincristine, dactinomycin, and doxorubicin with or without radiation therapy or observation only to see how well they work in treating patients undergoing surgery for newly diagnosed stage I, stage II, or stage III Wilms' tumor.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1200/jco.2017.73.7999 ; https://doi.org/10.1200/jco.18.01972</t>
+    <t>https://doi.org/10.1200/jco.2017.73.7999 https://doi.org/10.1200/jco.18.01972</t>
   </si>
   <si>
     <t>808</t>
@@ -8252,7 +8252,7 @@
     <t>This collection contains data from the Children's Oncology Group (COG) Clinical Trial NCT00274937, "Radiation Therapy, Amifostine, and Chemotherapy in Treating Young Patients With Newly Diagnosed Nasopharyngeal Cancer". Principal Investigator: Carlos Rodriguez-Galindo, MD. It was sponsored by NCI and performed by the Children's Oncology Group under study number ARAR0331. This phase III trial is studying how well radiation therapy, amifostine, and chemotherapy work in treating young patients with newly diagnosed nasopharyngeal cancer. Radiation therapy uses high-energy x-rays to kill tumor cells. Drugs, such as amifostine, may protect normal cells from the side effects of radiation therapy. Drugs used in chemotherapy, such as cisplatin and fluorouracil, work in different ways to stop the growth of tumor cells, either by killing the cells or by stopping them from dividing. Giving radiation therapy together with amifostine and chemotherapy may kill more tumor cells.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1200/jco.19.01692 ; https://doi.org/10.1200/jco.19.01276</t>
+    <t>https://doi.org/10.1200/jco.19.01692 https://doi.org/10.1200/jco.19.01276</t>
   </si>
   <si>
     <t>111</t>
@@ -8288,7 +8288,7 @@
     <t>Through this Clinical Sequencing Evidence-Generating Research (CSER2) with Enhanced Diversity project we will complete a trial (The Texas KidsCanSeq Study) comparing the results of targeted cancer panel sequencing versus genome-scale testing in pediatric cancer patients across diverse clinical settings. We will compare the targeted cancer panel to germline whole exome sequencing (WES) of unselected childhood cancer patients (n=1100) and WES, transcriptome sequencing and copy number array of FFPE tumor samples for the subset of patients with high-risk tumors (n=360). We will build on our success completing the CSER program BASIC3 exome sequencing trial (which included 60% Hispanic and African-American patients from a single large academic center) in this large multi-institutional study of an even more diverse patient population from five heterogeneous healthcare settings across Texas. The trial will be led by an experienced multi-PI team of Drs. Plon (medical geneticist), Parsons (pediatric oncologist) and McGuire (ethicist and health policy expert). We will assess clinical utility of these tests by measuring the frequency of diagnostic and/or actionable germline and tumor findings and the effect on treatment decisions (Aim 1). We will compare uptake by first degree relatives for familial genetic testing and recommended cancer surveillance by race, ethnicity and clinical settings (Aim 2). We will describe perceived utility (clinical, psychological, and pragmatic) by surveying and interviewing parents and participating pediatric oncologists (n=40) (Aim 3). Working with our pediatric cancer stakeholders, including advocates, BASIC3 study parents, and national organizations, we will create and evaluate the use of culturally sensitive educational materials, including videos in English and Spanish, improved integrated genomic test reports and counseling materials, and will compare in-person versus telemedicine exome results disclosure (Aim 4). Finally, we will provide data to guide future application of clinical genomics through three innovative pilot projects focused on health economics, decision support for cancer surveillance and whole genome sequencing (Aim 5). Baylor College of Medicine, Texas Children's Hospital, and our partner institutions across the state are ideally suited to conduct this study and play leadership roles in CSER2 consortium activities based on our longstanding pediatric oncology and cancer genetics expertise, extensive experience in CLIA-certified clinical germline and cancer genomic diagnostic testing, and a track record of scholarship in ethical and social implications of genomics and health disparities research.</t>
   </si>
   <si>
-    <t>https://doi.org/10.1007/s40271-021-00558-4 ; https://doi.org/10.1017/cts.2021.855</t>
+    <t>https://doi.org/10.1007/s40271-021-00558-4 https://doi.org/10.1017/cts.2021.855</t>
   </si>
   <si>
     <t>581</t>
@@ -8762,7 +8762,7 @@
     <t>mary@soe.ucsc.edu</t>
   </si>
   <si>
-    <t>https://doi.org/10.1101/326470 ; https://doi.org/10.1038/s41587-020-0546-8</t>
+    <t>https://doi.org/10.1101/326470 https://doi.org/10.1038/s41587-020-0546-8</t>
   </si>
   <si>
     <t>U24CA180951|Cloud Based Resource for Data Hosting, Visualization and Analysis Using UCSC Canc;U24CA210974|Visualization hub for genomics data exploration and translational discovery</t>

</xml_diff>

<commit_message>
ccdc datasets obj update
</commit_message>
<xml_diff>
--- a/InputFiles/CCDC_Datasets_20230413.xlsx
+++ b/InputFiles/CCDC_Datasets_20230413.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\May\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E204AD2E-088C-4122-94AA-4B0290183EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97A5ACE-A7B3-498D-9638-67B492CBB2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9227,8 +9227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A189" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B197" sqref="B197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -26861,7 +26861,7 @@
       </c>
     </row>
     <row r="199" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A199" t="s">
+      <c r="A199" s="4" t="s">
         <v>2662</v>
       </c>
       <c r="B199" t="s">
@@ -26950,7 +26950,7 @@
       </c>
     </row>
     <row r="200" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A200" t="s">
+      <c r="A200" s="4" t="s">
         <v>2674</v>
       </c>
       <c r="B200" t="s">
@@ -27039,7 +27039,7 @@
       </c>
     </row>
     <row r="201" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A201" t="s">
+      <c r="A201" s="4" t="s">
         <v>2684</v>
       </c>
       <c r="B201" t="s">
@@ -27128,7 +27128,7 @@
       </c>
     </row>
     <row r="202" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A202" t="s">
+      <c r="A202" s="4" t="s">
         <v>2696</v>
       </c>
       <c r="B202" t="s">
@@ -27217,7 +27217,7 @@
       </c>
     </row>
     <row r="203" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A203" t="s">
+      <c r="A203" s="4" t="s">
         <v>2707</v>
       </c>
       <c r="B203" t="s">
@@ -27306,7 +27306,7 @@
       </c>
     </row>
     <row r="204" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A204" t="s">
+      <c r="A204" s="4" t="s">
         <v>2719</v>
       </c>
       <c r="B204" t="s">

</xml_diff>